<commit_message>
"desecrate invade, devastate, discreet, evacuate, stroke, flock " added. excel updated.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="161">
   <si>
     <t>word</t>
   </si>
@@ -716,6 +716,186 @@
   </si>
   <si>
     <t>vimit</t>
+  </si>
+  <si>
+    <t>correlation</t>
+  </si>
+  <si>
+    <t>a connection between two ideas, facts etc, especially when one may be the cause of the other</t>
+  </si>
+  <si>
+    <t>there is a strong correlation between imcome and education</t>
+  </si>
+  <si>
+    <t>a strong correlation between urban deprivation and poor health</t>
+  </si>
+  <si>
+    <t>defy</t>
+  </si>
+  <si>
+    <t>to refuse to obey a law or rule, or refuse to do what someone in authority tells you to do</t>
+  </si>
+  <si>
+    <t>it's worng to defy the orders of superior officer.</t>
+  </si>
+  <si>
+    <t>Billy defied his mother, and smoked openly in the house.</t>
+  </si>
+  <si>
+    <t>superior</t>
+  </si>
+  <si>
+    <t> better, more powerful, more effective etc than a similar person or thing, especially one that you are competing against </t>
+  </si>
+  <si>
+    <t>Fletcher’s superior technique brought him victory.</t>
+  </si>
+  <si>
+    <t>Your computer is far superior to mine.</t>
+  </si>
+  <si>
+    <t>decontaminate</t>
+  </si>
+  <si>
+    <t>to remove a dangerous substance from somewhere</t>
+  </si>
+  <si>
+    <t>It may cost over $5 million to decontaminate the whole site.</t>
+  </si>
+  <si>
+    <t>it also helps decontaminate water and reduce the impact of floods.</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>the effect or influence that an event, situation etc has on someone or something</t>
+  </si>
+  <si>
+    <t>an international meeting to consider the environmental impacts of global warming</t>
+  </si>
+  <si>
+    <t>We need to assess the impact on climate change.</t>
+  </si>
+  <si>
+    <t>intention</t>
+  </si>
+  <si>
+    <t>a plan or desire to do something </t>
+  </si>
+  <si>
+    <t>I have no intention of retiring just yet.</t>
+  </si>
+  <si>
+    <t>you have the intention permanently to deprive me of the gasoline.</t>
+  </si>
+  <si>
+    <t>lucid</t>
+  </si>
+  <si>
+    <t>lure</t>
+  </si>
+  <si>
+    <t>to persuade someone to do something, especially something wrong or dangerous, by making it seem attractive or exciting</t>
+  </si>
+  <si>
+    <t>cheese is realy good lure for mice.</t>
+  </si>
+  <si>
+    <t>People may be lured into buying tickets by clever advertising.</t>
+  </si>
+  <si>
+    <t>expressed in a way that is clear and easy to understand</t>
+  </si>
+  <si>
+    <t>after finishing , she became lucid ,recognizedhim , agreed him.</t>
+  </si>
+  <si>
+    <t>You must write in a clear and lucid style.</t>
+  </si>
+  <si>
+    <t>desecrate</t>
+  </si>
+  <si>
+    <t>invade</t>
+  </si>
+  <si>
+    <t>devastate</t>
+  </si>
+  <si>
+    <t>evacuate</t>
+  </si>
+  <si>
+    <t>stroke</t>
+  </si>
+  <si>
+    <t>flock</t>
+  </si>
+  <si>
+    <t>to spoil or damage something holy or respected</t>
+  </si>
+  <si>
+    <t>Kelly's grave was also desecrated.</t>
+  </si>
+  <si>
+    <t>Most of the Egyptian tombs were desecrated and robbed.</t>
+  </si>
+  <si>
+    <t>to enter a country, town, or area using military force, in order to take control of it</t>
+  </si>
+  <si>
+    <t>Every summer, the town is invaded by tourists.</t>
+  </si>
+  <si>
+    <t>the invading army desectared this holy place when they camped.</t>
+  </si>
+  <si>
+    <t>each one of bombs can devastate a city.</t>
+  </si>
+  <si>
+    <t>to damage something very badly or completely</t>
+  </si>
+  <si>
+    <t>The city centre was devastated by the bomb.</t>
+  </si>
+  <si>
+    <t>discreet</t>
+  </si>
+  <si>
+    <t> careful about what you say or do, so that you do not offend, upset, or embarrass people or tell secrets</t>
+  </si>
+  <si>
+    <t>she is very discreed in giving her opinion</t>
+  </si>
+  <si>
+    <t>I stood back at a discreet distance.</t>
+  </si>
+  <si>
+    <t> to send people away from a dangerous place to a safe place</t>
+  </si>
+  <si>
+    <t>the official ordered the residents to evacuate.</t>
+  </si>
+  <si>
+    <t>During the war he was evacuated to Scotland.</t>
+  </si>
+  <si>
+    <t>if someone has a stroke, an artery (=tube carrying blood) in their brain suddenly bursts or becomes blocked, so that they may die or be unable to use some muscles</t>
+  </si>
+  <si>
+    <t>they intended to devastate the tower at a stroke.</t>
+  </si>
+  <si>
+    <t>I looked after my father after he had a stroke.</t>
+  </si>
+  <si>
+    <t> a group of sheep, goats, or birds</t>
+  </si>
+  <si>
+    <t>a flock of small birds</t>
+  </si>
+  <si>
+    <t>he keeps a flock of sheeps.</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,6 +1643,216 @@
         <v>94</v>
       </c>
     </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"beam brace classy consolation successor subtle stubborn admit spare" added.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="279">
   <si>
     <t>word</t>
   </si>
@@ -1145,6 +1145,111 @@
   </si>
   <si>
     <t>more people are going abroad for vacation.</t>
+  </si>
+  <si>
+    <t>beam</t>
+  </si>
+  <si>
+    <t>a long heavy piece of wood or metal used in building houses, bridges etc</t>
+  </si>
+  <si>
+    <t>Workers used steal beams to brace the roof.</t>
+  </si>
+  <si>
+    <t>Her head hit the beam and she slid down and hit her shoulder.</t>
+  </si>
+  <si>
+    <t>brace</t>
+  </si>
+  <si>
+    <t>brace yourself, to make something stronger by supporting it</t>
+  </si>
+  <si>
+    <t>The carpenter uses a brace to hold pieces of wood in place</t>
+  </si>
+  <si>
+    <t>Nancy braced herself for the inevitable arguments.</t>
+  </si>
+  <si>
+    <t>classy</t>
+  </si>
+  <si>
+    <t>stylish and sophisticated.</t>
+  </si>
+  <si>
+    <t>She took us to a very classy seafood restaurant in the old part of the city</t>
+  </si>
+  <si>
+    <t>The hotel is classy but relaxed.</t>
+  </si>
+  <si>
+    <t>consolation</t>
+  </si>
+  <si>
+    <t>the comfort received by a person after a loss or disappointment.</t>
+  </si>
+  <si>
+    <t>your company has been a great consolation to me.</t>
+  </si>
+  <si>
+    <t>The Church was the main consolation in a short and hard life.</t>
+  </si>
+  <si>
+    <t>successor</t>
+  </si>
+  <si>
+    <t>someone who takes a job or position previously held by someone else</t>
+  </si>
+  <si>
+    <t>His successor died after only 15 months in office.</t>
+  </si>
+  <si>
+    <t>subtle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> you have to be some more subtle with people.</t>
+  </si>
+  <si>
+    <t>not easy to notice or understand unless you pay careful attention</t>
+  </si>
+  <si>
+    <t>The pictures are similar, but there are subtle differences between them.</t>
+  </si>
+  <si>
+    <t>stubborn</t>
+  </si>
+  <si>
+    <t>determined not to change your mind, even when people think you are being unreasonable</t>
+  </si>
+  <si>
+    <t>he was too stubborn to admit that he was worng</t>
+  </si>
+  <si>
+    <t>Why are you so stubborn?</t>
+  </si>
+  <si>
+    <t>admit</t>
+  </si>
+  <si>
+    <t>to agree unwillingly that something is true or that someone else is right</t>
+  </si>
+  <si>
+    <t>You may not like her, but you have to admit that she’s good at her job.</t>
+  </si>
+  <si>
+    <t>I must admit, I didn’t actually do anything to help her.</t>
+  </si>
+  <si>
+    <t>spare</t>
+  </si>
+  <si>
+    <t>not being used or not needed at the present time</t>
+  </si>
+  <si>
+    <t>we have a spare in the trunk.</t>
+  </si>
+  <si>
+    <t>a spare bass guitar line.</t>
   </si>
 </sst>
 </file>
@@ -1517,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2442,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>225</v>
       </c>
@@ -2345,7 +2450,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>226</v>
       </c>
@@ -2353,7 +2458,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>228</v>
       </c>
@@ -2361,7 +2466,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>230</v>
       </c>
@@ -2369,7 +2474,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>232</v>
       </c>
@@ -2377,7 +2482,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>234</v>
       </c>
@@ -2385,7 +2490,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>236</v>
       </c>
@@ -2393,7 +2498,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>238</v>
       </c>
@@ -2401,7 +2506,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>240</v>
       </c>
@@ -2409,12 +2514,138 @@
         <v>241</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>242</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel and readme
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="325">
   <si>
     <t>word</t>
   </si>
@@ -1066,9 +1066,6 @@
     <t>oversee</t>
   </si>
   <si>
-    <t>appointe</t>
-  </si>
-  <si>
     <t>palate</t>
   </si>
   <si>
@@ -1090,21 +1087,12 @@
     <t>the care was narrow and impenetrable by humans.</t>
   </si>
   <si>
-    <t>impenetrable</t>
-  </si>
-  <si>
     <t>inform</t>
   </si>
   <si>
     <t>he informed us of the news.</t>
   </si>
   <si>
-    <t>deleterrius</t>
-  </si>
-  <si>
-    <t>children should be informed of the deleterrious effects of alcolol.</t>
-  </si>
-  <si>
     <t>involve</t>
   </si>
   <si>
@@ -1129,9 +1117,6 @@
     <t>that memory will abide in mind forever.</t>
   </si>
   <si>
-    <t>accomplishe</t>
-  </si>
-  <si>
     <t>he accomplished the dangerous mission</t>
   </si>
   <si>
@@ -1250,6 +1235,159 @@
   </si>
   <si>
     <t>a spare bass guitar line.</t>
+  </si>
+  <si>
+    <t>He soon regretted his hasty decision.</t>
+  </si>
+  <si>
+    <t>done in a hurry, especially with bad results</t>
+  </si>
+  <si>
+    <t>a plan or suggestion which is made formally to an official person or group, or the act of making it </t>
+  </si>
+  <si>
+    <t>the government’s proposals for regulation of the industry</t>
+  </si>
+  <si>
+    <t> to say or think that someone or something is responsible for something bad</t>
+  </si>
+  <si>
+    <t>Don’t blame me – it’s not my fault.</t>
+  </si>
+  <si>
+    <t> if the wind or a current of air blows, it moves</t>
+  </si>
+  <si>
+    <t>A cold breeze was blowing hard.</t>
+  </si>
+  <si>
+    <t>to shut and open your eyes quickly</t>
+  </si>
+  <si>
+    <t>I blinked as I came out into the sunlight.</t>
+  </si>
+  <si>
+    <t>a strong feeling of shame and sadness because you know that you have done something wrong</t>
+  </si>
+  <si>
+    <t>He used to buy them expensive presents, out of guilt.</t>
+  </si>
+  <si>
+    <t>something that is abundant exists or is available in large quantities so that there is more than enough</t>
+  </si>
+  <si>
+    <t>an abundant supply of fresh water</t>
+  </si>
+  <si>
+    <t> someone who sees a crime or an accident and can describe what happened</t>
+  </si>
+  <si>
+    <t>Police have appealed for witnesses to come forward.</t>
+  </si>
+  <si>
+    <t> information that is passed from one person to another about other people’s behaviour and private lives, often including unkind or untrue remarks</t>
+  </si>
+  <si>
+    <t>Here’s an interesting piece of gossip about Mrs Smith.</t>
+  </si>
+  <si>
+    <t>someone who talks about a religious subject in a public place, especially at a church</t>
+  </si>
+  <si>
+    <t>The preacher turned his volume up</t>
+  </si>
+  <si>
+    <t>to be in charge of a group of workers and check that a piece of work is done satisfactorily</t>
+  </si>
+  <si>
+    <t>A team leader was appointed to oversee the project.</t>
+  </si>
+  <si>
+    <t>appoint</t>
+  </si>
+  <si>
+    <t>to choose someone for a position or a job</t>
+  </si>
+  <si>
+    <t>officials appointed by the government</t>
+  </si>
+  <si>
+    <t>the sense of taste, and especially your ability to enjoy or judge food</t>
+  </si>
+  <si>
+    <t>a collection of dishes to tempt your palate</t>
+  </si>
+  <si>
+    <t> impossible to get through, see through, or get into</t>
+  </si>
+  <si>
+    <t>The trees formed a dark and impenetrable barrier.</t>
+  </si>
+  <si>
+    <t> to officially tell someone about something or give them information</t>
+  </si>
+  <si>
+    <t>They decided to inform the police</t>
+  </si>
+  <si>
+    <t>impenetrable != penetrate</t>
+  </si>
+  <si>
+    <t>deleterious</t>
+  </si>
+  <si>
+    <t>children should be informed of the deleterious effects of alcolol.</t>
+  </si>
+  <si>
+    <t>damaging or harmful</t>
+  </si>
+  <si>
+    <t>the deleterious effects of smoking</t>
+  </si>
+  <si>
+    <t>What will the job involve?</t>
+  </si>
+  <si>
+    <t>if an activity or situation involves something, that thing is part of it or a result of it.</t>
+  </si>
+  <si>
+    <t> ideas, opinions, statements etc that are not true or that seem very stupid</t>
+  </si>
+  <si>
+    <t>all this nonsense about health foods</t>
+  </si>
+  <si>
+    <t>if something or someone obsesses you, you think or worry about them all the time and you cannot think about anything else – used to show disapproval</t>
+  </si>
+  <si>
+    <t>A lot of young girls are obsessed by their weight.</t>
+  </si>
+  <si>
+    <t>accept or act in accordance with (a rule, decision, or recommendation).</t>
+  </si>
+  <si>
+    <t> Agreement to abide by the laws of the land is not enough</t>
+  </si>
+  <si>
+    <t>accomplish</t>
+  </si>
+  <si>
+    <t>to succeed in doing something, especially after trying very hard</t>
+  </si>
+  <si>
+    <t>We have accomplished all we set out to do.</t>
+  </si>
+  <si>
+    <t>to go somewhere with someone</t>
+  </si>
+  <si>
+    <t>Children under 14 must be accompanied by an adult.</t>
+  </si>
+  <si>
+    <t> in or to a foreign country</t>
+  </si>
+  <si>
+    <t>I’ve never lived abroad before.</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,20 +2468,32 @@
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="B51" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="C51" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="B52" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="C52" s="2" t="s">
         <v>199</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2354,298 +2504,424 @@
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="B54" s="2" t="s">
+        <v>278</v>
+      </c>
       <c r="C54" s="2" t="s">
         <v>203</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="B55" s="2" t="s">
+        <v>280</v>
+      </c>
       <c r="C55" s="2" t="s">
         <v>205</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="B56" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="C56" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>208</v>
       </c>
+      <c r="B57" s="2" t="s">
+        <v>284</v>
+      </c>
       <c r="C57" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="B58" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="C58" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="B59" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="C59" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="B60" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="C60" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="B61" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="C61" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="B62" s="2" t="s">
+        <v>294</v>
+      </c>
       <c r="C62" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="B64" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>223</v>
+      <c r="D64" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>227</v>
+      <c r="D66" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="B69" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="D69" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="B70" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="D70" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="B71" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>237</v>
+      <c r="D71" s="2" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>238</v>
+        <v>318</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
folk grumpy grapple inflation grudge hustle hostile construe added.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="345">
   <si>
     <t>word</t>
   </si>
@@ -1388,6 +1388,66 @@
   </si>
   <si>
     <t>I’ve never lived abroad before.</t>
+  </si>
+  <si>
+    <t>folk</t>
+  </si>
+  <si>
+    <t>a specific group of people, distinguished by common nationality, background, or style of life.</t>
+  </si>
+  <si>
+    <t>most of rich folk lives here.</t>
+  </si>
+  <si>
+    <t>Thanks to the folks at NBC.</t>
+  </si>
+  <si>
+    <t>grumpy</t>
+  </si>
+  <si>
+    <t>bad-tempered and easily annoyed</t>
+  </si>
+  <si>
+    <t>you are grumpy old man.</t>
+  </si>
+  <si>
+    <t>Come back and see me when you're less grumpy.</t>
+  </si>
+  <si>
+    <t>grapple</t>
+  </si>
+  <si>
+    <t>to fight or struggle with someone, holding them tightly.</t>
+  </si>
+  <si>
+    <t>the goverment is grappling with inflation.</t>
+  </si>
+  <si>
+    <t>Two men grappled with a guard at the door.</t>
+  </si>
+  <si>
+    <t>inflation</t>
+  </si>
+  <si>
+    <t>a continuing increase in prices, or the rate at which prices increase</t>
+  </si>
+  <si>
+    <t>Inflation is now at over 16%.</t>
+  </si>
+  <si>
+    <t>Too much government borrowing can lead to inflation.</t>
+  </si>
+  <si>
+    <t>grudge</t>
+  </si>
+  <si>
+    <t>a feeling of dislike for someone because you cannot forget that they harmed you in the past</t>
+  </si>
+  <si>
+    <t>I always feel she holds a grudge against me</t>
+  </si>
+  <si>
+    <t>Is there anyone who might have had a grudge against her?</t>
   </si>
 </sst>
 </file>
@@ -1760,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2924,6 +2984,76 @@
         <v>273</v>
       </c>
     </row>
+    <row r="84" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
hustle hostile construe added.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="357">
   <si>
     <t>word</t>
   </si>
@@ -1448,6 +1448,42 @@
   </si>
   <si>
     <t>Is there anyone who might have had a grudge against her?</t>
+  </si>
+  <si>
+    <t>hustle</t>
+  </si>
+  <si>
+    <t>to make someone move quickly, especially by pushing them roughly</t>
+  </si>
+  <si>
+    <t>I was hustled out of the building by a couple of security men.</t>
+  </si>
+  <si>
+    <t>they hustled to finish the task on time.</t>
+  </si>
+  <si>
+    <t>hostile</t>
+  </si>
+  <si>
+    <t>the boy feels hostile towards his father.</t>
+  </si>
+  <si>
+    <t>angry and deliberately unfriendly towards someone, and ready to argue with them</t>
+  </si>
+  <si>
+    <t>Southampton fans gave their former coach a hostile reception.</t>
+  </si>
+  <si>
+    <t>construe</t>
+  </si>
+  <si>
+    <t>to comprehend or explain the meaning or intention of; assign a meaning to; interpret.</t>
+  </si>
+  <si>
+    <t>comments that could be construed as sexist</t>
+  </si>
+  <si>
+    <t>they construcedmy words as cirtical and hostile.</t>
   </si>
 </sst>
 </file>
@@ -1820,10 +1856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,6 +3090,48 @@
         <v>344</v>
       </c>
     </row>
+    <row r="89" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
idiot, immunity ,narrow ,lane ,liable ,debt ,obliterate ,promenade added.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="389">
   <si>
     <t>word</t>
   </si>
@@ -1484,6 +1484,102 @@
   </si>
   <si>
     <t>they construcedmy words as cirtical and hostile.</t>
+  </si>
+  <si>
+    <t>idiot</t>
+  </si>
+  <si>
+    <t>a stupid person or someone who has done something stupid</t>
+  </si>
+  <si>
+    <t>I smile like an idiot when i'm talking to you.</t>
+  </si>
+  <si>
+    <t>It was all your fault, you idiot.</t>
+  </si>
+  <si>
+    <t>immunity</t>
+  </si>
+  <si>
+    <t>the state or right of being protected from particular laws or from unpleasant things</t>
+  </si>
+  <si>
+    <t>the caccine provides longer immunity against flu.</t>
+  </si>
+  <si>
+    <t>They were granted immunity from prosecution.</t>
+  </si>
+  <si>
+    <t>narrow</t>
+  </si>
+  <si>
+    <t>measuring only a small distance from one side to the other, especially in relation to the length</t>
+  </si>
+  <si>
+    <t>a long narrow road</t>
+  </si>
+  <si>
+    <t>The stairs were very narrow.</t>
+  </si>
+  <si>
+    <t>lane</t>
+  </si>
+  <si>
+    <t>a narrow road in the countryside</t>
+  </si>
+  <si>
+    <t>the police opened a lane through the crowd and let us pass.</t>
+  </si>
+  <si>
+    <t>a quiet country lane</t>
+  </si>
+  <si>
+    <t>liable</t>
+  </si>
+  <si>
+    <t>legally responsible for the cost of something</t>
+  </si>
+  <si>
+    <t>he claimed , he was not liable for his wife's debts.</t>
+  </si>
+  <si>
+    <t>You’re more liable to injury when you don’t get regular exercise.</t>
+  </si>
+  <si>
+    <t>debt</t>
+  </si>
+  <si>
+    <t>a sum of money that a person or organization owes</t>
+  </si>
+  <si>
+    <t>She had debts of over £100,000.</t>
+  </si>
+  <si>
+    <t>The band will be in debt to the record company for years.</t>
+  </si>
+  <si>
+    <t>obliterate</t>
+  </si>
+  <si>
+    <t>to destroy something completely so that nothing remains</t>
+  </si>
+  <si>
+    <t>the bomb nearly obliterate the city.</t>
+  </si>
+  <si>
+    <t>Hiroshima was nearly obliterated by the atomic bomb.</t>
+  </si>
+  <si>
+    <t>promenade</t>
+  </si>
+  <si>
+    <t>a wide road next to the beach, where people can walk for pleasure</t>
+  </si>
+  <si>
+    <t>we look a promenade along the canal after sunday dinner</t>
+  </si>
+  <si>
+    <t>This pier was not a promenade for me.</t>
   </si>
 </sst>
 </file>
@@ -1856,10 +1952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:D91"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,7 +3214,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>353</v>
       </c>
@@ -3130,6 +3226,118 @@
       </c>
       <c r="D91" s="2" t="s">
         <v>356</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>373</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall, scatter and scratch added.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="401">
   <si>
     <t>word</t>
   </si>
@@ -1580,6 +1580,42 @@
   </si>
   <si>
     <t>This pier was not a promenade for me.</t>
+  </si>
+  <si>
+    <t>fall</t>
+  </si>
+  <si>
+    <t>to move or drop down from a higher position to a lower position</t>
+  </si>
+  <si>
+    <t>The book fell from his hands.</t>
+  </si>
+  <si>
+    <t>the tree falls.</t>
+  </si>
+  <si>
+    <t>scatter</t>
+  </si>
+  <si>
+    <t>if someone scatters a lot of things, or if they scatter, they are thrown or dropped over a wide area in an irregular way</t>
+  </si>
+  <si>
+    <t>the wind scattered the dry fallen leaves.</t>
+  </si>
+  <si>
+    <t>Scatter the onions over the fish.</t>
+  </si>
+  <si>
+    <t>scratch</t>
+  </si>
+  <si>
+    <t>to rub your skin with your nails because it feels uncomfortable</t>
+  </si>
+  <si>
+    <t>the cat scratched the living room carpet.</t>
+  </si>
+  <si>
+    <t>John yawned and scratched his leg.</t>
   </si>
 </sst>
 </file>
@@ -1952,10 +1988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3340,6 +3376,48 @@
         <v>388</v>
       </c>
     </row>
+    <row r="100" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"severity sensation smuggle slope soak" added. this is last update.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="421">
   <si>
     <t>word</t>
   </si>
@@ -1616,6 +1616,66 @@
   </si>
   <si>
     <t>John yawned and scratched his leg.</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>severe problems, injuries, illnesses etc are very bad or very serious</t>
+  </si>
+  <si>
+    <t>he risk and severity of sunborn depend on he body's natural skin color.</t>
+  </si>
+  <si>
+    <t>His injuries were quite severe.</t>
+  </si>
+  <si>
+    <t>sensation</t>
+  </si>
+  <si>
+    <t>a feeling that you get from one of your five senses, especially the sense of touch</t>
+  </si>
+  <si>
+    <t>I experienced no sensation in my left foot.</t>
+  </si>
+  <si>
+    <t>One sign of a heart attack is a tingling sensation in the left arm.</t>
+  </si>
+  <si>
+    <t>smuggle</t>
+  </si>
+  <si>
+    <t>to take something or someone illegally from one country to another</t>
+  </si>
+  <si>
+    <t>if you try to smuggle drug you are stupid.</t>
+  </si>
+  <si>
+    <t>The guns were smuggled across the border.</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>a surface of which one end or side is at a higher level than another; a rising or falling surface.</t>
+  </si>
+  <si>
+    <t>the house builders slopped the roof...</t>
+  </si>
+  <si>
+    <t>the roof should have a slope sufficient for proper drainage</t>
+  </si>
+  <si>
+    <t>soak</t>
+  </si>
+  <si>
+    <t>if you soak something, or if you let it soak, you keep it covered with a liquid for a period of time, especially in order to make it softer or easier to clean</t>
+  </si>
+  <si>
+    <t>Soak the clothes in cold water.</t>
+  </si>
+  <si>
+    <t>soak the beans overnight in water</t>
   </si>
 </sst>
 </file>
@@ -1988,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,6 +3478,76 @@
         <v>400</v>
       </c>
     </row>
+    <row r="103" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"severity, sensation, smuggle, slope, soak" added. this is last update.
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="421">
   <si>
     <t>word</t>
   </si>
@@ -1616,6 +1616,66 @@
   </si>
   <si>
     <t>John yawned and scratched his leg.</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>severe problems, injuries, illnesses etc are very bad or very serious</t>
+  </si>
+  <si>
+    <t>he risk and severity of sunborn depend on he body's natural skin color.</t>
+  </si>
+  <si>
+    <t>His injuries were quite severe.</t>
+  </si>
+  <si>
+    <t>sensation</t>
+  </si>
+  <si>
+    <t>a feeling that you get from one of your five senses, especially the sense of touch</t>
+  </si>
+  <si>
+    <t>I experienced no sensation in my left foot.</t>
+  </si>
+  <si>
+    <t>One sign of a heart attack is a tingling sensation in the left arm.</t>
+  </si>
+  <si>
+    <t>smuggle</t>
+  </si>
+  <si>
+    <t>to take something or someone illegally from one country to another</t>
+  </si>
+  <si>
+    <t>if you try to smuggle drug you are stupid.</t>
+  </si>
+  <si>
+    <t>The guns were smuggled across the border.</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>a surface of which one end or side is at a higher level than another; a rising or falling surface.</t>
+  </si>
+  <si>
+    <t>the house builders slopped the roof...</t>
+  </si>
+  <si>
+    <t>the roof should have a slope sufficient for proper drainage</t>
+  </si>
+  <si>
+    <t>soak</t>
+  </si>
+  <si>
+    <t>if you soak something, or if you let it soak, you keep it covered with a liquid for a period of time, especially in order to make it softer or easier to clean</t>
+  </si>
+  <si>
+    <t>Soak the clothes in cold water.</t>
+  </si>
+  <si>
+    <t>soak the beans overnight in water</t>
   </si>
 </sst>
 </file>
@@ -1988,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,6 +3478,76 @@
         <v>400</v>
       </c>
     </row>
+    <row r="103" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>